<commit_message>
Update to capturing mosul case
</commit_message>
<xml_diff>
--- a/static/sample/SNA/CapturingMosulCase.xlsx
+++ b/static/sample/SNA/CapturingMosulCase.xlsx
@@ -2970,7 +2970,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3040,6 +3040,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3058,8 +3072,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3083,7 +3099,9 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3399,9 +3417,9 @@
   <dimension ref="A1:Q316"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A307" sqref="A307"/>
+      <selection pane="bottomLeft" activeCell="A308" sqref="A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12016,7 +12034,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added resilience measure UI aesthetics, added tooltips to SNA UI, added new hardcoded SNA attribute pairs
</commit_message>
<xml_diff>
--- a/static/sample/SNA/CapturingMosulCase.xlsx
+++ b/static/sample/SNA/CapturingMosulCase.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-36580" yWindow="-5780" windowWidth="25600" windowHeight="14320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sheet 2017" sheetId="1" r:id="rId1"/>
     <sheet name="Attribute" sheetId="2" r:id="rId2"/>
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -807,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -823,13 +823,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2941,29 +2943,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U50"/>
+  <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U7" sqref="U7:U16"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="18" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="4" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="4" style="16" customWidth="1"/>
+    <col min="7" max="7" width="4" style="18" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4" style="16" customWidth="1"/>
-    <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="15" max="15" width="4" customWidth="1"/>
-    <col min="17" max="17" width="4" customWidth="1"/>
-    <col min="19" max="19" width="4" customWidth="1"/>
+    <col min="9" max="9" width="4" style="18" customWidth="1"/>
+    <col min="11" max="11" width="4" style="17" customWidth="1"/>
+    <col min="13" max="13" width="4" style="17" customWidth="1"/>
+    <col min="15" max="15" width="4" style="17" customWidth="1"/>
+    <col min="17" max="17" width="4" style="17" customWidth="1"/>
+    <col min="18" max="18" width="9" customWidth="1"/>
+    <col min="19" max="19" width="4" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2973,55 +2976,55 @@
       <c r="B1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="19" t="s">
         <v>187</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="16" t="s">
         <v>187</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="16" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3032,29 +3035,65 @@
       <c r="B2" t="s">
         <v>188</v>
       </c>
+      <c r="C2" s="17">
+        <f t="shared" ref="C2:C50" ca="1" si="0">RAND()</f>
+        <v>0.80646429590604873</v>
+      </c>
       <c r="D2" t="s">
         <v>189</v>
       </c>
+      <c r="E2" s="17">
+        <f t="shared" ref="E2:E50" ca="1" si="1">RAND()</f>
+        <v>0.54042062981722738</v>
+      </c>
       <c r="F2" t="s">
         <v>190</v>
       </c>
+      <c r="G2" s="17">
+        <f t="shared" ref="G2:G50" ca="1" si="2">RAND()</f>
+        <v>0.55808727368441535</v>
+      </c>
       <c r="H2" t="s">
         <v>191</v>
       </c>
+      <c r="I2" s="17">
+        <f t="shared" ref="I2:I50" ca="1" si="3">RAND()</f>
+        <v>0.64885965031705206</v>
+      </c>
       <c r="J2" t="s">
         <v>192</v>
       </c>
+      <c r="K2" s="17">
+        <f t="shared" ref="K2:K50" ca="1" si="4">RAND()</f>
+        <v>0.18331112451993592</v>
+      </c>
       <c r="L2" t="s">
         <v>193</v>
       </c>
+      <c r="M2" s="17">
+        <f t="shared" ref="M2:M50" ca="1" si="5">RAND()</f>
+        <v>0.3854522436464406</v>
+      </c>
       <c r="N2" t="s">
         <v>194</v>
       </c>
+      <c r="O2" s="17">
+        <f t="shared" ref="O2:O50" ca="1" si="6">RAND()</f>
+        <v>0.9677771477267435</v>
+      </c>
       <c r="P2" t="s">
         <v>195</v>
       </c>
+      <c r="Q2" s="17">
+        <f t="shared" ref="Q2:Q50" ca="1" si="7">RAND()</f>
+        <v>0.17144668080433556</v>
+      </c>
       <c r="R2" t="s">
         <v>196</v>
+      </c>
+      <c r="S2" s="17">
+        <f ca="1">RAND()</f>
+        <v>0.87449255651276248</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -3064,29 +3103,65 @@
       <c r="B3" t="s">
         <v>188</v>
       </c>
+      <c r="C3" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55920898049223067</v>
+      </c>
       <c r="D3" t="s">
         <v>189</v>
       </c>
+      <c r="E3" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2771173567412587</v>
+      </c>
       <c r="F3" t="s">
         <v>190</v>
       </c>
+      <c r="G3" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.77416169957448178</v>
+      </c>
       <c r="H3" t="s">
         <v>191</v>
       </c>
+      <c r="I3" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.93604801839436302</v>
+      </c>
       <c r="J3" t="s">
         <v>192</v>
       </c>
+      <c r="K3" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.29329667443981478</v>
+      </c>
       <c r="L3" t="s">
         <v>193</v>
       </c>
+      <c r="M3" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.75391199704103173</v>
+      </c>
       <c r="N3" t="s">
         <v>194</v>
       </c>
+      <c r="O3" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.88746430398739773</v>
+      </c>
       <c r="P3" t="s">
         <v>195</v>
       </c>
+      <c r="Q3" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.76252758592532899</v>
+      </c>
       <c r="R3" t="s">
         <v>196</v>
+      </c>
+      <c r="S3" s="17">
+        <f ca="1">RAND()</f>
+        <v>0.15629756510957993</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -3096,29 +3171,65 @@
       <c r="B4" t="s">
         <v>188</v>
       </c>
+      <c r="C4" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69795035942523964</v>
+      </c>
       <c r="D4" t="s">
         <v>189</v>
       </c>
+      <c r="E4" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34316173406240114</v>
+      </c>
       <c r="F4" t="s">
         <v>190</v>
       </c>
+      <c r="G4" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.56438211030025498</v>
+      </c>
       <c r="H4" t="s">
         <v>191</v>
       </c>
+      <c r="I4" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26449577062503793</v>
+      </c>
       <c r="J4" t="s">
         <v>192</v>
       </c>
+      <c r="K4" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.42692187336355836</v>
+      </c>
       <c r="L4" t="s">
         <v>193</v>
       </c>
+      <c r="M4" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.88719145046628778</v>
+      </c>
       <c r="N4" t="s">
         <v>194</v>
       </c>
+      <c r="O4" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.82402037631447145</v>
+      </c>
       <c r="P4" t="s">
         <v>195</v>
       </c>
+      <c r="Q4" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.48132048474569433</v>
+      </c>
       <c r="R4" t="s">
         <v>196</v>
+      </c>
+      <c r="S4" s="17">
+        <f t="shared" ref="S4:S50" ca="1" si="8">RAND()</f>
+        <v>0.40671385486655254</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -3128,29 +3239,65 @@
       <c r="B5" t="s">
         <v>188</v>
       </c>
+      <c r="C5" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.4856987949402098E-2</v>
+      </c>
       <c r="D5" t="s">
         <v>189</v>
       </c>
+      <c r="E5" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19143568467777405</v>
+      </c>
       <c r="F5" t="s">
         <v>190</v>
       </c>
+      <c r="G5" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.17197266910564335</v>
+      </c>
       <c r="H5" t="s">
         <v>191</v>
       </c>
+      <c r="I5" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.95229872863606635</v>
+      </c>
       <c r="J5" t="s">
         <v>192</v>
       </c>
+      <c r="K5" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.8996873944264987E-2</v>
+      </c>
       <c r="L5" t="s">
         <v>193</v>
       </c>
+      <c r="M5" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.88679456848278126</v>
+      </c>
       <c r="N5" t="s">
         <v>194</v>
       </c>
+      <c r="O5" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.80715749736873998</v>
+      </c>
       <c r="P5" t="s">
         <v>195</v>
       </c>
+      <c r="Q5" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.82612744474780753</v>
+      </c>
       <c r="R5" t="s">
         <v>196</v>
+      </c>
+      <c r="S5" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.50663883603771465</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -3160,29 +3307,65 @@
       <c r="B6" t="s">
         <v>188</v>
       </c>
+      <c r="C6" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65642285285237223</v>
+      </c>
       <c r="D6" t="s">
         <v>189</v>
       </c>
+      <c r="E6" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44899231204304191</v>
+      </c>
       <c r="F6" t="s">
         <v>190</v>
       </c>
+      <c r="G6" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.5730038116609536</v>
+      </c>
       <c r="H6" t="s">
         <v>191</v>
       </c>
+      <c r="I6" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53815884662596503</v>
+      </c>
       <c r="J6" t="s">
         <v>192</v>
       </c>
+      <c r="K6" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.44974155969122498</v>
+      </c>
       <c r="L6" t="s">
         <v>193</v>
       </c>
+      <c r="M6" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.62677460980594468</v>
+      </c>
       <c r="N6" t="s">
         <v>194</v>
       </c>
+      <c r="O6" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.57845609226646144</v>
+      </c>
       <c r="P6" t="s">
         <v>195</v>
       </c>
+      <c r="Q6" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>6.0426788136680565E-2</v>
+      </c>
       <c r="R6" t="s">
         <v>196</v>
+      </c>
+      <c r="S6" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.32052787106886804</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -3192,29 +3375,65 @@
       <c r="B7" t="s">
         <v>188</v>
       </c>
+      <c r="C7" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.81182271540070761</v>
+      </c>
       <c r="D7" t="s">
         <v>189</v>
       </c>
+      <c r="E7" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39078171515722993</v>
+      </c>
       <c r="F7" t="s">
         <v>190</v>
       </c>
+      <c r="G7" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.32584175941032834</v>
+      </c>
       <c r="H7" t="s">
         <v>191</v>
       </c>
+      <c r="I7" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.62374870745689737</v>
+      </c>
       <c r="J7" t="s">
         <v>192</v>
       </c>
+      <c r="K7" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.85336677589076337</v>
+      </c>
       <c r="L7" t="s">
         <v>193</v>
       </c>
+      <c r="M7" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.7268819940111571E-2</v>
+      </c>
       <c r="N7" t="s">
         <v>194</v>
       </c>
+      <c r="O7" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.70274488648298394</v>
+      </c>
       <c r="P7" t="s">
         <v>195</v>
       </c>
+      <c r="Q7" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.47398865949878899</v>
+      </c>
       <c r="R7" t="s">
         <v>196</v>
+      </c>
+      <c r="S7" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.14945149808777636</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -3224,31 +3443,67 @@
       <c r="B8" t="s">
         <v>188</v>
       </c>
+      <c r="C8" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80288456927649032</v>
+      </c>
       <c r="D8" t="s">
         <v>189</v>
       </c>
+      <c r="E8" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6536606883240434E-2</v>
+      </c>
       <c r="F8" t="s">
         <v>190</v>
       </c>
+      <c r="G8" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.45103070545392154</v>
+      </c>
       <c r="H8" t="s">
         <v>191</v>
       </c>
+      <c r="I8" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.44544279792860808</v>
+      </c>
       <c r="J8" t="s">
         <v>192</v>
       </c>
+      <c r="K8" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.49659949613302579</v>
+      </c>
       <c r="L8" t="s">
         <v>193</v>
       </c>
+      <c r="M8" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.36782001443114709</v>
+      </c>
       <c r="N8" t="s">
         <v>194</v>
       </c>
+      <c r="O8" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.92717301119461315</v>
+      </c>
       <c r="P8" t="s">
         <v>195</v>
       </c>
+      <c r="Q8" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.99648628395839878</v>
+      </c>
       <c r="R8" t="s">
         <v>196</v>
       </c>
-      <c r="U8" s="17"/>
+      <c r="S8" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.32968146060362702</v>
+      </c>
+      <c r="U8" s="15"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3257,31 +3512,67 @@
       <c r="B9" t="s">
         <v>188</v>
       </c>
+      <c r="C9" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0029042733834683E-2</v>
+      </c>
       <c r="D9" t="s">
         <v>189</v>
       </c>
+      <c r="E9" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16027678549762414</v>
+      </c>
       <c r="F9" t="s">
         <v>190</v>
       </c>
+      <c r="G9" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.64133684814222558</v>
+      </c>
       <c r="H9" t="s">
         <v>191</v>
       </c>
+      <c r="I9" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.43971607146407643</v>
+      </c>
       <c r="J9" t="s">
         <v>192</v>
       </c>
+      <c r="K9" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>9.4528422652427779E-2</v>
+      </c>
       <c r="L9" t="s">
         <v>193</v>
       </c>
+      <c r="M9" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.2949220257501266</v>
+      </c>
       <c r="N9" t="s">
         <v>194</v>
       </c>
+      <c r="O9" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.33896645644393952</v>
+      </c>
       <c r="P9" t="s">
         <v>195</v>
       </c>
+      <c r="Q9" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.75696162349812979</v>
+      </c>
       <c r="R9" t="s">
         <v>196</v>
       </c>
-      <c r="U9" s="17"/>
+      <c r="S9" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.32519978539608152</v>
+      </c>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -3290,31 +3581,67 @@
       <c r="B10" t="s">
         <v>188</v>
       </c>
+      <c r="C10" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.44312938634405308</v>
+      </c>
       <c r="D10" t="s">
         <v>189</v>
       </c>
+      <c r="E10" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70884387207853439</v>
+      </c>
       <c r="F10" t="s">
         <v>190</v>
       </c>
+      <c r="G10" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.97322023577911687</v>
+      </c>
       <c r="H10" t="s">
         <v>191</v>
       </c>
+      <c r="I10" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.231795674378383</v>
+      </c>
       <c r="J10" t="s">
         <v>192</v>
       </c>
+      <c r="K10" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.53651516056205995</v>
+      </c>
       <c r="L10" t="s">
         <v>193</v>
       </c>
+      <c r="M10" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.70243186738600538</v>
+      </c>
       <c r="N10" t="s">
         <v>194</v>
       </c>
+      <c r="O10" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.688108013195466</v>
+      </c>
       <c r="P10" t="s">
         <v>195</v>
       </c>
+      <c r="Q10" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.46576982688685942</v>
+      </c>
       <c r="R10" t="s">
         <v>196</v>
       </c>
-      <c r="U10" s="17"/>
+      <c r="S10" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.35169209795723844</v>
+      </c>
+      <c r="U10" s="15"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
@@ -3323,31 +3650,67 @@
       <c r="B11" t="s">
         <v>188</v>
       </c>
+      <c r="C11" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56835889467024436</v>
+      </c>
       <c r="D11" t="s">
         <v>189</v>
       </c>
+      <c r="E11" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>9.7768890629949423E-2</v>
+      </c>
       <c r="F11" t="s">
         <v>190</v>
       </c>
+      <c r="G11" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.58084747548688487</v>
+      </c>
       <c r="H11" t="s">
         <v>191</v>
       </c>
+      <c r="I11" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.56799106330778459</v>
+      </c>
       <c r="J11" t="s">
         <v>192</v>
       </c>
+      <c r="K11" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.81519025826350033</v>
+      </c>
       <c r="L11" t="s">
         <v>193</v>
       </c>
+      <c r="M11" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.2426335267180687</v>
+      </c>
       <c r="N11" t="s">
         <v>194</v>
       </c>
+      <c r="O11" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.40797060271060925</v>
+      </c>
       <c r="P11" t="s">
         <v>195</v>
       </c>
+      <c r="Q11" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.74352183540387951</v>
+      </c>
       <c r="R11" t="s">
         <v>196</v>
       </c>
-      <c r="U11" s="17"/>
+      <c r="S11" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.5253562769126946</v>
+      </c>
+      <c r="U11" s="15"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
@@ -3356,31 +3719,67 @@
       <c r="B12" t="s">
         <v>188</v>
       </c>
+      <c r="C12" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.42317318900115597</v>
+      </c>
       <c r="D12" t="s">
         <v>189</v>
       </c>
+      <c r="E12" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64040622992367024</v>
+      </c>
       <c r="F12" t="s">
         <v>190</v>
       </c>
+      <c r="G12" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.789514123968134E-2</v>
+      </c>
       <c r="H12" t="s">
         <v>191</v>
       </c>
+      <c r="I12" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.76789485208041253</v>
+      </c>
       <c r="J12" t="s">
         <v>192</v>
       </c>
+      <c r="K12" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.86669516690100634</v>
+      </c>
       <c r="L12" t="s">
         <v>193</v>
       </c>
+      <c r="M12" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.87392091929340543</v>
+      </c>
       <c r="N12" t="s">
         <v>194</v>
       </c>
+      <c r="O12" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.9764785276974618</v>
+      </c>
       <c r="P12" t="s">
         <v>195</v>
       </c>
+      <c r="Q12" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.64185155783817327</v>
+      </c>
       <c r="R12" t="s">
         <v>196</v>
       </c>
-      <c r="U12" s="17"/>
+      <c r="S12" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.97445873129158433</v>
+      </c>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -3389,31 +3788,67 @@
       <c r="B13" t="s">
         <v>188</v>
       </c>
+      <c r="C13" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.3798679056637728E-2</v>
+      </c>
       <c r="D13" t="s">
         <v>189</v>
       </c>
+      <c r="E13" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32321078323434749</v>
+      </c>
       <c r="F13" t="s">
         <v>190</v>
       </c>
+      <c r="G13" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.94036911966809833</v>
+      </c>
       <c r="H13" t="s">
         <v>191</v>
       </c>
+      <c r="I13" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.71655546025402739</v>
+      </c>
       <c r="J13" t="s">
         <v>192</v>
       </c>
+      <c r="K13" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.86791268946661482</v>
+      </c>
       <c r="L13" t="s">
         <v>193</v>
       </c>
+      <c r="M13" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74084448736669539</v>
+      </c>
       <c r="N13" t="s">
         <v>194</v>
       </c>
+      <c r="O13" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.24284136407924595</v>
+      </c>
       <c r="P13" t="s">
         <v>195</v>
       </c>
+      <c r="Q13" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.62880388601128268</v>
+      </c>
       <c r="R13" t="s">
         <v>196</v>
       </c>
-      <c r="U13" s="17"/>
+      <c r="S13" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.88086818683721013</v>
+      </c>
+      <c r="U13" s="15"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -3422,31 +3857,67 @@
       <c r="B14" t="s">
         <v>188</v>
       </c>
+      <c r="C14" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9215227614399764E-2</v>
+      </c>
       <c r="D14" t="s">
         <v>189</v>
       </c>
+      <c r="E14" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9166428057161714</v>
+      </c>
       <c r="F14" t="s">
         <v>190</v>
       </c>
+      <c r="G14" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.97523800871185229</v>
+      </c>
       <c r="H14" t="s">
         <v>191</v>
       </c>
+      <c r="I14" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.45114760180249558</v>
+      </c>
       <c r="J14" t="s">
         <v>192</v>
       </c>
+      <c r="K14" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.78284459065839751</v>
+      </c>
       <c r="L14" t="s">
         <v>193</v>
       </c>
+      <c r="M14" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.547779762357685</v>
+      </c>
       <c r="N14" t="s">
         <v>194</v>
       </c>
+      <c r="O14" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>4.9864223132184526E-2</v>
+      </c>
       <c r="P14" t="s">
         <v>195</v>
       </c>
+      <c r="Q14" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.3184488231254177E-2</v>
+      </c>
       <c r="R14" t="s">
         <v>196</v>
       </c>
-      <c r="U14" s="17"/>
+      <c r="S14" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.66205456280412689</v>
+      </c>
+      <c r="U14" s="15"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -3455,31 +3926,67 @@
       <c r="B15" t="s">
         <v>188</v>
       </c>
+      <c r="C15" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48861008786593896</v>
+      </c>
       <c r="D15" t="s">
         <v>189</v>
       </c>
+      <c r="E15" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14266191772064296</v>
+      </c>
       <c r="F15" t="s">
         <v>190</v>
       </c>
+      <c r="G15" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.99135585795675851</v>
+      </c>
       <c r="H15" t="s">
         <v>191</v>
       </c>
+      <c r="I15" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.52373915200753973</v>
+      </c>
       <c r="J15" t="s">
         <v>192</v>
       </c>
+      <c r="K15" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.21164598208464636</v>
+      </c>
       <c r="L15" t="s">
         <v>193</v>
       </c>
+      <c r="M15" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.98201631448194349</v>
+      </c>
       <c r="N15" t="s">
         <v>194</v>
       </c>
+      <c r="O15" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.19274908900670229</v>
+      </c>
       <c r="P15" t="s">
         <v>195</v>
       </c>
+      <c r="Q15" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.90030182519572566</v>
+      </c>
       <c r="R15" t="s">
         <v>196</v>
       </c>
-      <c r="U15" s="17"/>
+      <c r="S15" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.84857851695120634</v>
+      </c>
+      <c r="U15" s="15"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3488,1119 +3995,2382 @@
       <c r="B16" t="s">
         <v>188</v>
       </c>
+      <c r="C16" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1509993941012</v>
+      </c>
       <c r="D16" t="s">
         <v>189</v>
       </c>
+      <c r="E16" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79921248590139649</v>
+      </c>
       <c r="F16" t="s">
         <v>190</v>
       </c>
+      <c r="G16" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.66208375010132925</v>
+      </c>
       <c r="H16" t="s">
         <v>191</v>
       </c>
+      <c r="I16" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26296199540388598</v>
+      </c>
       <c r="J16" t="s">
         <v>192</v>
       </c>
+      <c r="K16" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.3787136501587105</v>
+      </c>
       <c r="L16" t="s">
         <v>193</v>
       </c>
+      <c r="M16" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.75113412260396117</v>
+      </c>
       <c r="N16" t="s">
         <v>194</v>
       </c>
+      <c r="O16" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.57856697741885899</v>
+      </c>
       <c r="P16" t="s">
         <v>195</v>
       </c>
+      <c r="Q16" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.6454159420450124</v>
+      </c>
       <c r="R16" t="s">
         <v>196</v>
       </c>
-      <c r="U16" s="17"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S16" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.73870656277108138</v>
+      </c>
+      <c r="U16" s="15"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
       <c r="B17" t="s">
         <v>188</v>
       </c>
+      <c r="C17" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96583855723337164</v>
+      </c>
       <c r="D17" t="s">
         <v>189</v>
       </c>
+      <c r="E17" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2135374889554299</v>
+      </c>
       <c r="F17" t="s">
         <v>190</v>
       </c>
+      <c r="G17" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.8309629122442939E-2</v>
+      </c>
       <c r="H17" t="s">
         <v>191</v>
       </c>
+      <c r="I17" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.43976481810446832</v>
+      </c>
       <c r="J17" t="s">
         <v>192</v>
       </c>
+      <c r="K17" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.38363665014208903</v>
+      </c>
       <c r="L17" t="s">
         <v>193</v>
       </c>
+      <c r="M17" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.59412608566042924</v>
+      </c>
       <c r="N17" t="s">
         <v>194</v>
       </c>
+      <c r="O17" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.96546437303734234</v>
+      </c>
       <c r="P17" t="s">
         <v>195</v>
       </c>
+      <c r="Q17" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.93520864709571661</v>
+      </c>
       <c r="R17" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.41159710560894236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>188</v>
       </c>
+      <c r="C18" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49007351630761409</v>
+      </c>
       <c r="D18" t="s">
         <v>189</v>
       </c>
+      <c r="E18" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60153219712765349</v>
+      </c>
       <c r="F18" t="s">
         <v>190</v>
       </c>
+      <c r="G18" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.98893065673467961</v>
+      </c>
       <c r="H18" t="s">
         <v>191</v>
       </c>
+      <c r="I18" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.0842512805578925E-2</v>
+      </c>
       <c r="J18" t="s">
         <v>192</v>
       </c>
+      <c r="K18" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.80290700870889831</v>
+      </c>
       <c r="L18" t="s">
         <v>193</v>
       </c>
+      <c r="M18" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.50902168595188924</v>
+      </c>
       <c r="N18" t="s">
         <v>194</v>
       </c>
+      <c r="O18" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.70837895750044655</v>
+      </c>
       <c r="P18" t="s">
         <v>195</v>
       </c>
+      <c r="Q18" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.52671587968560585</v>
+      </c>
       <c r="R18" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.64694968958766275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
       <c r="B19" t="s">
         <v>188</v>
       </c>
+      <c r="C19" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.65241807082498E-2</v>
+      </c>
       <c r="D19" t="s">
         <v>189</v>
       </c>
+      <c r="E19" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.56922773485468892</v>
+      </c>
       <c r="F19" t="s">
         <v>190</v>
       </c>
+      <c r="G19" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.6715054154450346E-2</v>
+      </c>
       <c r="H19" t="s">
         <v>191</v>
       </c>
+      <c r="I19" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.19965636577236534</v>
+      </c>
       <c r="J19" t="s">
         <v>192</v>
       </c>
+      <c r="K19" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.31739746577174266</v>
+      </c>
       <c r="L19" t="s">
         <v>193</v>
       </c>
+      <c r="M19" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.10185660805890695</v>
+      </c>
       <c r="N19" t="s">
         <v>194</v>
       </c>
+      <c r="O19" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.49458110729221827</v>
+      </c>
       <c r="P19" t="s">
         <v>195</v>
       </c>
+      <c r="Q19" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.87421124997713751</v>
+      </c>
       <c r="R19" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S19" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.2377398803037275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>188</v>
       </c>
+      <c r="C20" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69611480211482524</v>
+      </c>
       <c r="D20" t="s">
         <v>189</v>
       </c>
+      <c r="E20" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.9668367177326394E-2</v>
+      </c>
       <c r="F20" t="s">
         <v>190</v>
       </c>
+      <c r="G20" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15471800959078719</v>
+      </c>
       <c r="H20" t="s">
         <v>191</v>
       </c>
+      <c r="I20" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.5420689177310456</v>
+      </c>
       <c r="J20" t="s">
         <v>192</v>
       </c>
+      <c r="K20" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.64477901432961293</v>
+      </c>
       <c r="L20" t="s">
         <v>193</v>
       </c>
+      <c r="M20" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57523512900464946</v>
+      </c>
       <c r="N20" t="s">
         <v>194</v>
       </c>
+      <c r="O20" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.42004836651848565</v>
+      </c>
       <c r="P20" t="s">
         <v>195</v>
       </c>
+      <c r="Q20" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.90173592247204792</v>
+      </c>
       <c r="R20" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S20" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.55938905186789856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>75</v>
       </c>
       <c r="B21" t="s">
         <v>188</v>
       </c>
+      <c r="C21" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7928004038840832E-3</v>
+      </c>
       <c r="D21" t="s">
         <v>189</v>
       </c>
+      <c r="E21" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49472500872946579</v>
+      </c>
       <c r="F21" t="s">
         <v>190</v>
       </c>
+      <c r="G21" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.39127344861129609</v>
+      </c>
       <c r="H21" t="s">
         <v>191</v>
       </c>
+      <c r="I21" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.478540065319916</v>
+      </c>
       <c r="J21" t="s">
         <v>192</v>
       </c>
+      <c r="K21" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.96783038044071257</v>
+      </c>
       <c r="L21" t="s">
         <v>193</v>
       </c>
+      <c r="M21" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.71641411602161909</v>
+      </c>
       <c r="N21" t="s">
         <v>194</v>
       </c>
+      <c r="O21" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.98008065755947049</v>
+      </c>
       <c r="P21" t="s">
         <v>195</v>
       </c>
+      <c r="Q21" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.71878397193944521</v>
+      </c>
       <c r="R21" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S21" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.64535130579040068</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>188</v>
       </c>
+      <c r="C22" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17085513203760627</v>
+      </c>
       <c r="D22" t="s">
         <v>189</v>
       </c>
+      <c r="E22" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64987974569224316</v>
+      </c>
       <c r="F22" t="s">
         <v>190</v>
       </c>
+      <c r="G22" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.48763360157709501</v>
+      </c>
       <c r="H22" t="s">
         <v>191</v>
       </c>
+      <c r="I22" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53665548996984469</v>
+      </c>
       <c r="J22" t="s">
         <v>192</v>
       </c>
+      <c r="K22" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.46881583175281427</v>
+      </c>
       <c r="L22" t="s">
         <v>193</v>
       </c>
+      <c r="M22" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.41259985688422518</v>
+      </c>
       <c r="N22" t="s">
         <v>194</v>
       </c>
+      <c r="O22" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.95237036195673164</v>
+      </c>
       <c r="P22" t="s">
         <v>195</v>
       </c>
+      <c r="Q22" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.89931794353676486</v>
+      </c>
       <c r="R22" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S22" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.7872331617786329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>188</v>
       </c>
+      <c r="C23" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68208290200994748</v>
+      </c>
       <c r="D23" t="s">
         <v>189</v>
       </c>
+      <c r="E23" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73240453111527337</v>
+      </c>
       <c r="F23" t="s">
         <v>190</v>
       </c>
+      <c r="G23" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15117584949400265</v>
+      </c>
       <c r="H23" t="s">
         <v>191</v>
       </c>
+      <c r="I23" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.74486430475888898</v>
+      </c>
       <c r="J23" t="s">
         <v>192</v>
       </c>
+      <c r="K23" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.85180725904397825</v>
+      </c>
       <c r="L23" t="s">
         <v>193</v>
       </c>
+      <c r="M23" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.21304245104142971</v>
+      </c>
       <c r="N23" t="s">
         <v>194</v>
       </c>
+      <c r="O23" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.52523747202252435</v>
+      </c>
       <c r="P23" t="s">
         <v>195</v>
       </c>
+      <c r="Q23" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.92107449015870713</v>
+      </c>
       <c r="R23" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S23" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.54844119030520189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>83</v>
       </c>
       <c r="B24" t="s">
         <v>188</v>
       </c>
+      <c r="C24" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18911934666755259</v>
+      </c>
       <c r="D24" t="s">
         <v>189</v>
       </c>
+      <c r="E24" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17336485901285748</v>
+      </c>
       <c r="F24" t="s">
         <v>190</v>
       </c>
+      <c r="G24" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.73374923983381135</v>
+      </c>
       <c r="H24" t="s">
         <v>191</v>
       </c>
+      <c r="I24" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53815261016573046</v>
+      </c>
       <c r="J24" t="s">
         <v>192</v>
       </c>
+      <c r="K24" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.89830905016962637</v>
+      </c>
       <c r="L24" t="s">
         <v>193</v>
       </c>
+      <c r="M24" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.61527955462323647</v>
+      </c>
       <c r="N24" t="s">
         <v>194</v>
       </c>
+      <c r="O24" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.72343603348767127</v>
+      </c>
       <c r="P24" t="s">
         <v>195</v>
       </c>
+      <c r="Q24" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.69875435022157872</v>
+      </c>
       <c r="R24" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S24" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.64359294603750483</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>188</v>
       </c>
+      <c r="C25" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21389307726304918</v>
+      </c>
       <c r="D25" t="s">
         <v>189</v>
       </c>
+      <c r="E25" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51885871739307499</v>
+      </c>
       <c r="F25" t="s">
         <v>190</v>
       </c>
+      <c r="G25" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.81910807498244953</v>
+      </c>
       <c r="H25" t="s">
         <v>191</v>
       </c>
+      <c r="I25" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.63319666028184574</v>
+      </c>
       <c r="J25" t="s">
         <v>192</v>
       </c>
+      <c r="K25" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.40914685198709777</v>
+      </c>
       <c r="L25" t="s">
         <v>193</v>
       </c>
+      <c r="M25" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.74373328183731213</v>
+      </c>
       <c r="N25" t="s">
         <v>194</v>
       </c>
+      <c r="O25" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.49280839582789771</v>
+      </c>
       <c r="P25" t="s">
         <v>195</v>
       </c>
+      <c r="Q25" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.683067154303755E-2</v>
+      </c>
       <c r="R25" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S25" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.3244604628743493E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>188</v>
       </c>
+      <c r="C26" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.7449661019020288E-2</v>
+      </c>
       <c r="D26" t="s">
         <v>189</v>
       </c>
+      <c r="E26" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15660403280040625</v>
+      </c>
       <c r="F26" t="s">
         <v>190</v>
       </c>
+      <c r="G26" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15214005401361497</v>
+      </c>
       <c r="H26" t="s">
         <v>191</v>
       </c>
+      <c r="I26" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15924042701711916</v>
+      </c>
       <c r="J26" t="s">
         <v>192</v>
       </c>
+      <c r="K26" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.52883629623439132</v>
+      </c>
       <c r="L26" t="s">
         <v>193</v>
       </c>
+      <c r="M26" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.17761714433653197</v>
+      </c>
       <c r="N26" t="s">
         <v>194</v>
       </c>
+      <c r="O26" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.63077343497290106</v>
+      </c>
       <c r="P26" t="s">
         <v>195</v>
       </c>
+      <c r="Q26" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.29201028741923862</v>
+      </c>
       <c r="R26" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S26" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.1622832144320534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>188</v>
       </c>
+      <c r="C27" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.43984913889906141</v>
+      </c>
       <c r="D27" t="s">
         <v>189</v>
       </c>
+      <c r="E27" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53583662861256343</v>
+      </c>
       <c r="F27" t="s">
         <v>190</v>
       </c>
+      <c r="G27" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.77928907179462081</v>
+      </c>
       <c r="H27" t="s">
         <v>191</v>
       </c>
+      <c r="I27" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.59756257363209453</v>
+      </c>
       <c r="J27" t="s">
         <v>192</v>
       </c>
+      <c r="K27" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.63790923691507406</v>
+      </c>
       <c r="L27" t="s">
         <v>193</v>
       </c>
+      <c r="M27" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.33960784523447418</v>
+      </c>
       <c r="N27" t="s">
         <v>194</v>
       </c>
+      <c r="O27" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>7.5430898209203678E-2</v>
+      </c>
       <c r="P27" t="s">
         <v>195</v>
       </c>
+      <c r="Q27" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.38657416630322261</v>
+      </c>
       <c r="R27" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S27" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>4.447660463820402E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B28" t="s">
         <v>188</v>
       </c>
+      <c r="C28" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51054282306487231</v>
+      </c>
       <c r="D28" t="s">
         <v>189</v>
       </c>
+      <c r="E28" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.2681898279642878E-3</v>
+      </c>
       <c r="F28" t="s">
         <v>190</v>
       </c>
+      <c r="G28" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.88684979643282946</v>
+      </c>
       <c r="H28" t="s">
         <v>191</v>
       </c>
+      <c r="I28" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.18577880514049283</v>
+      </c>
       <c r="J28" t="s">
         <v>192</v>
       </c>
+      <c r="K28" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.75341141932505118</v>
+      </c>
       <c r="L28" t="s">
         <v>193</v>
       </c>
+      <c r="M28" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.33408936276920109</v>
+      </c>
       <c r="N28" t="s">
         <v>194</v>
       </c>
+      <c r="O28" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.32030769913643686</v>
+      </c>
       <c r="P28" t="s">
         <v>195</v>
       </c>
+      <c r="Q28" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.41062210807520794</v>
+      </c>
       <c r="R28" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S28" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.55263791341928314</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B29" t="s">
         <v>188</v>
       </c>
+      <c r="C29" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3740803344817677</v>
+      </c>
       <c r="D29" t="s">
         <v>189</v>
       </c>
+      <c r="E29" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.0924557795241649E-2</v>
+      </c>
       <c r="F29" t="s">
         <v>190</v>
       </c>
+      <c r="G29" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.74714437363342356</v>
+      </c>
       <c r="H29" t="s">
         <v>191</v>
       </c>
+      <c r="I29" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>6.9649078365269679E-2</v>
+      </c>
       <c r="J29" t="s">
         <v>192</v>
       </c>
+      <c r="K29" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.64509084594613952</v>
+      </c>
       <c r="L29" t="s">
         <v>193</v>
       </c>
+      <c r="M29" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.90237071990161599</v>
+      </c>
       <c r="N29" t="s">
         <v>194</v>
       </c>
+      <c r="O29" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.17710821998682302</v>
+      </c>
       <c r="P29" t="s">
         <v>195</v>
       </c>
+      <c r="Q29" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.55717160949409439</v>
+      </c>
       <c r="R29" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S29" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.49410031248855746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B30" t="s">
         <v>188</v>
       </c>
+      <c r="C30" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82863416952629276</v>
+      </c>
       <c r="D30" t="s">
         <v>189</v>
       </c>
+      <c r="E30" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.97068596108599148</v>
+      </c>
       <c r="F30" t="s">
         <v>190</v>
       </c>
+      <c r="G30" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.70064962927873331</v>
+      </c>
       <c r="H30" t="s">
         <v>191</v>
       </c>
+      <c r="I30" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.65662967614653778</v>
+      </c>
       <c r="J30" t="s">
         <v>192</v>
       </c>
+      <c r="K30" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.46862519631939448</v>
+      </c>
       <c r="L30" t="s">
         <v>193</v>
       </c>
+      <c r="M30" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.4412974994340626</v>
+      </c>
       <c r="N30" t="s">
         <v>194</v>
       </c>
+      <c r="O30" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.75155791845756903</v>
+      </c>
       <c r="P30" t="s">
         <v>195</v>
       </c>
+      <c r="Q30" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.76216597129677655</v>
+      </c>
       <c r="R30" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S30" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.1546396703853166E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>101</v>
       </c>
       <c r="B31" t="s">
         <v>188</v>
       </c>
+      <c r="C31" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.7875208137724314E-2</v>
+      </c>
       <c r="D31" t="s">
         <v>189</v>
       </c>
+      <c r="E31" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.24881498669054714</v>
+      </c>
       <c r="F31" t="s">
         <v>190</v>
       </c>
+      <c r="G31" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.94458016624093155</v>
+      </c>
       <c r="H31" t="s">
         <v>191</v>
       </c>
+      <c r="I31" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.21601381900454031</v>
+      </c>
       <c r="J31" t="s">
         <v>192</v>
       </c>
+      <c r="K31" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.15382014053855908</v>
+      </c>
       <c r="L31" t="s">
         <v>193</v>
       </c>
+      <c r="M31" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.8496733709759821E-2</v>
+      </c>
       <c r="N31" t="s">
         <v>194</v>
       </c>
+      <c r="O31" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.90724631356156449</v>
+      </c>
       <c r="P31" t="s">
         <v>195</v>
       </c>
+      <c r="Q31" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.59520046410841876</v>
+      </c>
       <c r="R31" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S31" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.29317079299927573</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>188</v>
       </c>
+      <c r="C32" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72987519291398006</v>
+      </c>
       <c r="D32" t="s">
         <v>189</v>
       </c>
+      <c r="E32" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.54047770510018489</v>
+      </c>
       <c r="F32" t="s">
         <v>190</v>
       </c>
+      <c r="G32" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22120609324128515</v>
+      </c>
       <c r="H32" t="s">
         <v>191</v>
       </c>
+      <c r="I32" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.34044724781630153</v>
+      </c>
       <c r="J32" t="s">
         <v>192</v>
       </c>
+      <c r="K32" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.5500748491666454</v>
+      </c>
       <c r="L32" t="s">
         <v>193</v>
       </c>
+      <c r="M32" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.60874838956184474</v>
+      </c>
       <c r="N32" t="s">
         <v>194</v>
       </c>
+      <c r="O32" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.36332692592943383</v>
+      </c>
       <c r="P32" t="s">
         <v>195</v>
       </c>
+      <c r="Q32" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.46612817957763786</v>
+      </c>
       <c r="R32" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S32" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.13386495701538426</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>108</v>
       </c>
       <c r="B33" t="s">
         <v>188</v>
       </c>
+      <c r="C33" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0452722348171739E-2</v>
+      </c>
       <c r="D33" t="s">
         <v>189</v>
       </c>
+      <c r="E33" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91201000284519229</v>
+      </c>
       <c r="F33" t="s">
         <v>190</v>
       </c>
+      <c r="G33" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.14957827557414283</v>
+      </c>
       <c r="H33" t="s">
         <v>191</v>
       </c>
+      <c r="I33" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.477158314748518</v>
+      </c>
       <c r="J33" t="s">
         <v>192</v>
       </c>
+      <c r="K33" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.35034570083062777</v>
+      </c>
       <c r="L33" t="s">
         <v>193</v>
       </c>
+      <c r="M33" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.25168150705326242</v>
+      </c>
       <c r="N33" t="s">
         <v>194</v>
       </c>
+      <c r="O33" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.97489562627453352</v>
+      </c>
       <c r="P33" t="s">
         <v>195</v>
       </c>
+      <c r="Q33" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.26901083694788386</v>
+      </c>
       <c r="R33" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S33" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.74261768337722356</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>111</v>
       </c>
       <c r="B34" t="s">
         <v>188</v>
       </c>
+      <c r="C34" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.42570382571871546</v>
+      </c>
       <c r="D34" t="s">
         <v>189</v>
       </c>
+      <c r="E34" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.71004004077258442</v>
+      </c>
       <c r="F34" t="s">
         <v>190</v>
       </c>
+      <c r="G34" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.87907508324931705</v>
+      </c>
       <c r="H34" t="s">
         <v>191</v>
       </c>
+      <c r="I34" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.68657144453328334</v>
+      </c>
       <c r="J34" t="s">
         <v>192</v>
       </c>
+      <c r="K34" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.97434269407332941</v>
+      </c>
       <c r="L34" t="s">
         <v>193</v>
       </c>
+      <c r="M34" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.1069492715414031</v>
+      </c>
       <c r="N34" t="s">
         <v>194</v>
       </c>
+      <c r="O34" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.21804711911968933</v>
+      </c>
       <c r="P34" t="s">
         <v>195</v>
       </c>
+      <c r="Q34" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.96689311288852586</v>
+      </c>
       <c r="R34" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S34" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>8.8640427138918398E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>116</v>
       </c>
       <c r="B35" t="s">
         <v>188</v>
       </c>
+      <c r="C35" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1656870624720428E-2</v>
+      </c>
       <c r="D35" t="s">
         <v>189</v>
       </c>
+      <c r="E35" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.57345469212194222</v>
+      </c>
       <c r="F35" t="s">
         <v>190</v>
       </c>
+      <c r="G35" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.5382702302426017E-2</v>
+      </c>
       <c r="H35" t="s">
         <v>191</v>
       </c>
+      <c r="I35" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.95079226025370178</v>
+      </c>
       <c r="J35" t="s">
         <v>192</v>
       </c>
+      <c r="K35" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.47676796028655899</v>
+      </c>
       <c r="L35" t="s">
         <v>193</v>
       </c>
+      <c r="M35" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.736373835038088E-2</v>
+      </c>
       <c r="N35" t="s">
         <v>194</v>
       </c>
+      <c r="O35" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.73983709757824634</v>
+      </c>
       <c r="P35" t="s">
         <v>195</v>
       </c>
+      <c r="Q35" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>8.3532198387933576E-2</v>
+      </c>
       <c r="R35" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S35" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.14947007876347695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>120</v>
       </c>
       <c r="B36" t="s">
         <v>188</v>
       </c>
+      <c r="C36" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51270763251337459</v>
+      </c>
       <c r="D36" t="s">
         <v>189</v>
       </c>
+      <c r="E36" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14570797342762087</v>
+      </c>
       <c r="F36" t="s">
         <v>190</v>
       </c>
+      <c r="G36" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3663583120043018</v>
+      </c>
       <c r="H36" t="s">
         <v>191</v>
       </c>
+      <c r="I36" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.96455547724977808</v>
+      </c>
       <c r="J36" t="s">
         <v>192</v>
       </c>
+      <c r="K36" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.2281129573454672E-2</v>
+      </c>
       <c r="L36" t="s">
         <v>193</v>
       </c>
+      <c r="M36" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.23075802079853969</v>
+      </c>
       <c r="N36" t="s">
         <v>194</v>
       </c>
+      <c r="O36" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.94788882732438851</v>
+      </c>
       <c r="P36" t="s">
         <v>195</v>
       </c>
+      <c r="Q36" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.52700847947158369</v>
+      </c>
       <c r="R36" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S36" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.93545887884011136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>123</v>
       </c>
       <c r="B37" t="s">
         <v>188</v>
       </c>
+      <c r="C37" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32762128245077071</v>
+      </c>
       <c r="D37" t="s">
         <v>189</v>
       </c>
+      <c r="E37" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5233740835315962</v>
+      </c>
       <c r="F37" t="s">
         <v>190</v>
       </c>
+      <c r="G37" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.52978809343642641</v>
+      </c>
       <c r="H37" t="s">
         <v>191</v>
       </c>
+      <c r="I37" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.19529043946609503</v>
+      </c>
       <c r="J37" t="s">
         <v>192</v>
       </c>
+      <c r="K37" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.91556339773290352</v>
+      </c>
       <c r="L37" t="s">
         <v>193</v>
       </c>
+      <c r="M37" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.86490434372651459</v>
+      </c>
       <c r="N37" t="s">
         <v>194</v>
       </c>
+      <c r="O37" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26297849585450694</v>
+      </c>
       <c r="P37" t="s">
         <v>195</v>
       </c>
+      <c r="Q37" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.29008040956499659</v>
+      </c>
       <c r="R37" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S37" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.60673846689930067</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>188</v>
       </c>
+      <c r="C38" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61827128567826928</v>
+      </c>
       <c r="D38" t="s">
         <v>189</v>
       </c>
+      <c r="E38" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16239260307604397</v>
+      </c>
       <c r="F38" t="s">
         <v>190</v>
       </c>
+      <c r="G38" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.13653681426269726</v>
+      </c>
       <c r="H38" t="s">
         <v>191</v>
       </c>
+      <c r="I38" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.29328449765206299</v>
+      </c>
       <c r="J38" t="s">
         <v>192</v>
       </c>
+      <c r="K38" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.87955422599706401</v>
+      </c>
       <c r="L38" t="s">
         <v>193</v>
       </c>
+      <c r="M38" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.56719793640177729</v>
+      </c>
       <c r="N38" t="s">
         <v>194</v>
       </c>
+      <c r="O38" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.32296549501191218</v>
+      </c>
       <c r="P38" t="s">
         <v>195</v>
       </c>
+      <c r="Q38" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.98169839407471404</v>
+      </c>
       <c r="R38" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S38" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.99744491126567292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>132</v>
       </c>
       <c r="B39" t="s">
         <v>188</v>
       </c>
+      <c r="C39" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59825357793372158</v>
+      </c>
       <c r="D39" t="s">
         <v>189</v>
       </c>
+      <c r="E39" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18533560926969772</v>
+      </c>
       <c r="F39" t="s">
         <v>190</v>
       </c>
+      <c r="G39" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3046951298467383</v>
+      </c>
       <c r="H39" t="s">
         <v>191</v>
       </c>
+      <c r="I39" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53904986326292337</v>
+      </c>
       <c r="J39" t="s">
         <v>192</v>
       </c>
+      <c r="K39" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.76810728820911189</v>
+      </c>
       <c r="L39" t="s">
         <v>193</v>
       </c>
+      <c r="M39" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.99396920285930102</v>
+      </c>
       <c r="N39" t="s">
         <v>194</v>
       </c>
+      <c r="O39" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.89296634312807921</v>
+      </c>
       <c r="P39" t="s">
         <v>195</v>
       </c>
+      <c r="Q39" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.83020545710392335</v>
+      </c>
       <c r="R39" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S39" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.19948915255476107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>137</v>
       </c>
       <c r="B40" t="s">
         <v>188</v>
       </c>
+      <c r="C40" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10894412350618665</v>
+      </c>
       <c r="D40" t="s">
         <v>189</v>
       </c>
+      <c r="E40" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.97502742653830232</v>
+      </c>
       <c r="F40" t="s">
         <v>190</v>
       </c>
+      <c r="G40" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8296410363009579E-2</v>
+      </c>
       <c r="H40" t="s">
         <v>191</v>
       </c>
+      <c r="I40" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.35624259691908788</v>
+      </c>
       <c r="J40" t="s">
         <v>192</v>
       </c>
+      <c r="K40" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12896435444501164</v>
+      </c>
       <c r="L40" t="s">
         <v>193</v>
       </c>
+      <c r="M40" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.66095695348886263</v>
+      </c>
       <c r="N40" t="s">
         <v>194</v>
       </c>
+      <c r="O40" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.17154894928675657</v>
+      </c>
       <c r="P40" t="s">
         <v>195</v>
       </c>
+      <c r="Q40" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.49882192918356061</v>
+      </c>
       <c r="R40" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S40" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.12497171712022626</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>188</v>
       </c>
+      <c r="C41" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6708609941004E-2</v>
+      </c>
       <c r="D41" t="s">
         <v>189</v>
       </c>
+      <c r="E41" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95348538544802386</v>
+      </c>
       <c r="F41" t="s">
         <v>190</v>
       </c>
+      <c r="G41" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.8439019944408939E-2</v>
+      </c>
       <c r="H41" t="s">
         <v>191</v>
       </c>
+      <c r="I41" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15322175955214057</v>
+      </c>
       <c r="J41" t="s">
         <v>192</v>
       </c>
+      <c r="K41" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.83336292639108189</v>
+      </c>
       <c r="L41" t="s">
         <v>193</v>
       </c>
+      <c r="M41" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>6.0486302464626718E-2</v>
+      </c>
       <c r="N41" t="s">
         <v>194</v>
       </c>
+      <c r="O41" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.55507708861485716</v>
+      </c>
       <c r="P41" t="s">
         <v>195</v>
       </c>
+      <c r="Q41" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.39932564829760053</v>
+      </c>
       <c r="R41" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S41" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.90612621098368895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>146</v>
       </c>
       <c r="B42" t="s">
         <v>188</v>
       </c>
+      <c r="C42" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17671702583479743</v>
+      </c>
       <c r="D42" t="s">
         <v>189</v>
       </c>
+      <c r="E42" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92997674185733858</v>
+      </c>
       <c r="F42" t="s">
         <v>190</v>
       </c>
+      <c r="G42" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.46759228605348757</v>
+      </c>
       <c r="H42" t="s">
         <v>191</v>
       </c>
+      <c r="I42" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>7.8525731686246325E-2</v>
+      </c>
       <c r="J42" t="s">
         <v>192</v>
       </c>
+      <c r="K42" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.8231854703175624</v>
+      </c>
       <c r="L42" t="s">
         <v>193</v>
       </c>
+      <c r="M42" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.2167850822899875E-2</v>
+      </c>
       <c r="N42" t="s">
         <v>194</v>
       </c>
+      <c r="O42" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.37184827582731506</v>
+      </c>
       <c r="P42" t="s">
         <v>195</v>
       </c>
+      <c r="Q42" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.2461511066068065</v>
+      </c>
       <c r="R42" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S42" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.34574939367144886</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>149</v>
       </c>
       <c r="B43" t="s">
         <v>188</v>
       </c>
+      <c r="C43" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.3257526688006909E-2</v>
+      </c>
       <c r="D43" t="s">
         <v>189</v>
       </c>
+      <c r="E43" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87069333922957326</v>
+      </c>
       <c r="F43" t="s">
         <v>190</v>
       </c>
+      <c r="G43" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.67422654959867512</v>
+      </c>
       <c r="H43" t="s">
         <v>191</v>
       </c>
+      <c r="I43" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14561994669682898</v>
+      </c>
       <c r="J43" t="s">
         <v>192</v>
       </c>
+      <c r="K43" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.87561114959111852</v>
+      </c>
       <c r="L43" t="s">
         <v>193</v>
       </c>
+      <c r="M43" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.1786873164111823</v>
+      </c>
       <c r="N43" t="s">
         <v>194</v>
       </c>
+      <c r="O43" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.37141071113362656</v>
+      </c>
       <c r="P43" t="s">
         <v>195</v>
       </c>
+      <c r="Q43" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.35179186833183906</v>
+      </c>
       <c r="R43" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S43" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.40312940679713405</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>154</v>
       </c>
       <c r="B44" t="s">
         <v>188</v>
       </c>
+      <c r="C44" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94929882734837401</v>
+      </c>
       <c r="D44" t="s">
         <v>189</v>
       </c>
+      <c r="E44" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69008765979159625</v>
+      </c>
       <c r="F44" t="s">
         <v>190</v>
       </c>
+      <c r="G44" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.32301942603245859</v>
+      </c>
       <c r="H44" t="s">
         <v>191</v>
       </c>
+      <c r="I44" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1329878176131335</v>
+      </c>
       <c r="J44" t="s">
         <v>192</v>
       </c>
+      <c r="K44" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.59621977985301655</v>
+      </c>
       <c r="L44" t="s">
         <v>193</v>
       </c>
+      <c r="M44" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.88229357881834902</v>
+      </c>
       <c r="N44" t="s">
         <v>194</v>
       </c>
+      <c r="O44" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.65902804140720783</v>
+      </c>
       <c r="P44" t="s">
         <v>195</v>
       </c>
+      <c r="Q44" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.28159386534717512</v>
+      </c>
       <c r="R44" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S44" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.39176257064638742</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>157</v>
       </c>
       <c r="B45" t="s">
         <v>188</v>
       </c>
+      <c r="C45" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56936121628617031</v>
+      </c>
       <c r="D45" t="s">
         <v>189</v>
       </c>
+      <c r="E45" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.3176016987755998E-3</v>
+      </c>
       <c r="F45" t="s">
         <v>190</v>
       </c>
+      <c r="G45" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.54508541290502133</v>
+      </c>
       <c r="H45" t="s">
         <v>191</v>
       </c>
+      <c r="I45" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.72034852930003268</v>
+      </c>
       <c r="J45" t="s">
         <v>192</v>
       </c>
+      <c r="K45" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.91640219376423637</v>
+      </c>
       <c r="L45" t="s">
         <v>193</v>
       </c>
+      <c r="M45" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.92897759555172765</v>
+      </c>
       <c r="N45" t="s">
         <v>194</v>
       </c>
+      <c r="O45" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.39857123656091387</v>
+      </c>
       <c r="P45" t="s">
         <v>195</v>
       </c>
+      <c r="Q45" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.6095976952301051</v>
+      </c>
       <c r="R45" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S45" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.83338233789293525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>160</v>
       </c>
       <c r="B46" t="s">
         <v>188</v>
       </c>
+      <c r="C46" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58689883971077861</v>
+      </c>
       <c r="D46" t="s">
         <v>189</v>
       </c>
+      <c r="E46" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7518549365322188</v>
+      </c>
       <c r="F46" t="s">
         <v>190</v>
       </c>
+      <c r="G46" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.36668718039503279</v>
+      </c>
       <c r="H46" t="s">
         <v>191</v>
       </c>
+      <c r="I46" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>7.8571886962589765E-2</v>
+      </c>
       <c r="J46" t="s">
         <v>192</v>
       </c>
+      <c r="K46" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.7891547070509826E-2</v>
+      </c>
       <c r="L46" t="s">
         <v>193</v>
       </c>
+      <c r="M46" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5937698765215752</v>
+      </c>
       <c r="N46" t="s">
         <v>194</v>
       </c>
+      <c r="O46" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26903581209657201</v>
+      </c>
       <c r="P46" t="s">
         <v>195</v>
       </c>
+      <c r="Q46" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.9144568349278358</v>
+      </c>
       <c r="R46" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S46" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.41006058188847727</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>163</v>
       </c>
       <c r="B47" t="s">
         <v>188</v>
       </c>
+      <c r="C47" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.77113015069724167</v>
+      </c>
       <c r="D47" t="s">
         <v>189</v>
       </c>
+      <c r="E47" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.7961467867955188E-2</v>
+      </c>
       <c r="F47" t="s">
         <v>190</v>
       </c>
+      <c r="G47" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.37698313537820027</v>
+      </c>
       <c r="H47" t="s">
         <v>191</v>
       </c>
+      <c r="I47" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.9888330398880949</v>
+      </c>
       <c r="J47" t="s">
         <v>192</v>
       </c>
+      <c r="K47" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.16736400771866877</v>
+      </c>
       <c r="L47" t="s">
         <v>193</v>
       </c>
+      <c r="M47" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.29885343322362046</v>
+      </c>
       <c r="N47" t="s">
         <v>194</v>
       </c>
+      <c r="O47" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.40633082325417613</v>
+      </c>
       <c r="P47" t="s">
         <v>195</v>
       </c>
+      <c r="Q47" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.94811253417913366</v>
+      </c>
       <c r="R47" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S47" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.20799100743744503</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>169</v>
       </c>
       <c r="B48" t="s">
         <v>188</v>
       </c>
+      <c r="C48" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50590753094834462</v>
+      </c>
       <c r="D48" t="s">
         <v>189</v>
       </c>
+      <c r="E48" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14205135273084912</v>
+      </c>
       <c r="F48" t="s">
         <v>190</v>
       </c>
+      <c r="G48" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.5084487112265026E-2</v>
+      </c>
       <c r="H48" t="s">
         <v>191</v>
       </c>
+      <c r="I48" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.25802121588096305</v>
+      </c>
       <c r="J48" t="s">
         <v>192</v>
       </c>
+      <c r="K48" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.61616107972911038</v>
+      </c>
       <c r="L48" t="s">
         <v>193</v>
       </c>
+      <c r="M48" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.59591973357180372</v>
+      </c>
       <c r="N48" t="s">
         <v>194</v>
       </c>
+      <c r="O48" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.46448923780403928</v>
+      </c>
       <c r="P48" t="s">
         <v>195</v>
       </c>
+      <c r="Q48" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.5844713006882043</v>
+      </c>
       <c r="R48" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S48" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>9.6876731233309976E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>174</v>
       </c>
       <c r="B49" t="s">
         <v>188</v>
       </c>
+      <c r="C49" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8825495147875112</v>
+      </c>
       <c r="D49" t="s">
         <v>189</v>
       </c>
+      <c r="E49" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3551082300994638</v>
+      </c>
       <c r="F49" t="s">
         <v>190</v>
       </c>
+      <c r="G49" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4881871821479078E-2</v>
+      </c>
       <c r="H49" t="s">
         <v>191</v>
       </c>
+      <c r="I49" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.11489333325622297</v>
+      </c>
       <c r="J49" t="s">
         <v>192</v>
       </c>
+      <c r="K49" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.48970476316451594</v>
+      </c>
       <c r="L49" t="s">
         <v>193</v>
       </c>
+      <c r="M49" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.6527313655266922</v>
+      </c>
       <c r="N49" t="s">
         <v>194</v>
       </c>
+      <c r="O49" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.17902124128110086</v>
+      </c>
       <c r="P49" t="s">
         <v>195</v>
       </c>
+      <c r="Q49" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.50367203409913186</v>
+      </c>
       <c r="R49" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S49" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.86562062106299464</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>179</v>
       </c>
       <c r="B50" t="s">
         <v>188</v>
       </c>
+      <c r="C50" s="17">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74800489664668546</v>
+      </c>
       <c r="D50" t="s">
         <v>189</v>
       </c>
+      <c r="E50" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3759367830429815</v>
+      </c>
       <c r="F50" t="s">
         <v>190</v>
       </c>
+      <c r="G50" s="17">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.57910267708789043</v>
+      </c>
       <c r="H50" t="s">
         <v>191</v>
       </c>
+      <c r="I50" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.47680127421647167</v>
+      </c>
       <c r="J50" t="s">
         <v>192</v>
       </c>
+      <c r="K50" s="17">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.47195052879883548</v>
+      </c>
       <c r="L50" t="s">
         <v>193</v>
       </c>
+      <c r="M50" s="17">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.58028553474562661</v>
+      </c>
       <c r="N50" t="s">
         <v>194</v>
       </c>
+      <c r="O50" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.57443809227556397</v>
+      </c>
       <c r="P50" t="s">
         <v>195</v>
       </c>
+      <c r="Q50" s="17">
+        <f t="shared" ca="1" si="7"/>
+        <v>6.955749247698606E-2</v>
+      </c>
       <c r="R50" t="s">
         <v>196</v>
       </c>
+      <c r="S50" s="17">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.69540106564634141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N59" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>